<commit_message>
Empresa CaX/Gestion de Configuracion/SisCoTe_PGC.docx
Se añadio la lista de items con nomenclatura
</commit_message>
<xml_diff>
--- a/Empresa CaX/PROY_SisCoTe/Documentacion/Negocio/SisCoTe_LR.xlsx
+++ b/Empresa CaX/PROY_SisCoTe/Documentacion/Negocio/SisCoTe_LR.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
@@ -458,6 +458,81 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -467,78 +542,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -546,9 +549,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -824,7 +824,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -834,14 +834,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="42" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="21" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="60" customWidth="1"/>
     <col min="5" max="5" width="27.140625" customWidth="1"/>
@@ -851,16 +851,16 @@
   <sheetData>
     <row r="2" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -898,7 +898,7 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="22" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -924,7 +924,7 @@
       <c r="C6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -941,25 +941,25 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24">
+      <c r="A7" s="32">
         <v>2</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="36" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="34" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="7" t="s">
@@ -967,49 +967,49 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="46"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="40"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="47"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="41"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
       <c r="H9" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24">
+      <c r="A10" s="32">
         <v>4</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="10" t="s">
@@ -1017,25 +1017,25 @@
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="8" t="s">
         <v>42</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="C13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="23" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="9" t="s">
@@ -1067,25 +1067,25 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="35">
+      <c r="A14" s="29">
         <v>6</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="33" t="s">
         <v>8</v>
       </c>
       <c r="H14" s="5" t="s">
@@ -1093,37 +1093,37 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="36"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="36"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
       <c r="H16" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
       <c r="H17" s="7" t="s">
         <v>29</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="C18" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="22" t="s">
         <v>50</v>
       </c>
       <c r="E18" s="15" t="s">
@@ -1162,7 +1162,7 @@
       <c r="C19" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="22" t="s">
         <v>61</v>
       </c>
       <c r="E19" s="6" t="s">
@@ -1186,7 +1186,7 @@
       <c r="C20" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="22" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="6" t="s">
@@ -1210,7 +1210,7 @@
       <c r="C21" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="22" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="6" t="s">
@@ -1236,6 +1236,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C7:C9"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="A3:H3"/>
@@ -1252,12 +1258,6 @@
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="E10:E12"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C7:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>